<commit_message>
first decade is working; home page and phrases page reachable again
</commit_message>
<xml_diff>
--- a/lib/seeds/subcategories.xlsx
+++ b/lib/seeds/subcategories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dkolokolov/code/escapist-berlin/du_und_ich/lib/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D35DAAD-B554-5F4E-9F70-D24DCB11293A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B927BCA-E87E-4040-ADAD-19E7D293D10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5200" yWindow="1300" windowWidth="28040" windowHeight="17360" xr2:uid="{8D37ADAD-6A58-CA44-B564-CD4B0BD8DEF4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14160" xr2:uid="{8D37ADAD-6A58-CA44-B564-CD4B0BD8DEF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Alter</t>
-  </si>
-  <si>
-    <t>Korper merkmale</t>
   </si>
   <si>
     <t>Charakter</t>
@@ -447,7 +444,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -468,7 +465,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -484,7 +481,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -492,7 +489,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -500,7 +497,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -508,7 +505,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -516,7 +513,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -524,7 +521,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -532,7 +529,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -540,7 +537,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -556,7 +553,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -564,7 +561,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -572,7 +569,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -580,7 +577,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -588,7 +585,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -596,7 +593,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -604,7 +601,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -612,7 +609,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -620,7 +617,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -628,7 +625,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -636,7 +633,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -644,7 +641,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -652,7 +649,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25">
         <v>3</v>

</xml_diff>

<commit_message>
order and spelling of filters fixed
</commit_message>
<xml_diff>
--- a/lib/seeds/subcategories.xlsx
+++ b/lib/seeds/subcategories.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dkolokolov/code/escapist-berlin/du_und_ich/lib/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B927BCA-E87E-4040-ADAD-19E7D293D10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1F14C7-1588-0049-9B7F-80A66B3DF63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14160" xr2:uid="{8D37ADAD-6A58-CA44-B564-CD4B0BD8DEF4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -44,52 +44,49 @@
     <t>SUBCATEGORY</t>
   </si>
   <si>
-    <t>Alter</t>
-  </si>
-  <si>
-    <t>Charakter</t>
-  </si>
-  <si>
-    <t>Tribes</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>Hobbies</t>
-  </si>
-  <si>
-    <t>Job Bezeichnung</t>
-  </si>
-  <si>
     <t>Klasse</t>
   </si>
   <si>
-    <t>Körper Merkmale</t>
-  </si>
-  <si>
-    <t>Ethnie</t>
-  </si>
-  <si>
-    <t>Jobbezeichnung</t>
-  </si>
-  <si>
-    <t>Chat</t>
-  </si>
-  <si>
-    <t>Verabredung</t>
-  </si>
-  <si>
-    <t>Freunde</t>
-  </si>
-  <si>
-    <t>Vernetzung</t>
-  </si>
-  <si>
-    <t>Beziehung</t>
-  </si>
-  <si>
     <t>Nur Spaß</t>
+  </si>
+  <si>
+    <t>Alter </t>
+  </si>
+  <si>
+    <t>Körpertyp </t>
+  </si>
+  <si>
+    <t>Charakter </t>
+  </si>
+  <si>
+    <t>Ethnie </t>
+  </si>
+  <si>
+    <t>Tribes </t>
+  </si>
+  <si>
+    <t>Position </t>
+  </si>
+  <si>
+    <t>Hobbies </t>
+  </si>
+  <si>
+    <t>Jobbezeichnung </t>
+  </si>
+  <si>
+    <t>Chat </t>
+  </si>
+  <si>
+    <t>Verabredungen </t>
+  </si>
+  <si>
+    <t>Freunde </t>
+  </si>
+  <si>
+    <t>Vernetzung </t>
+  </si>
+  <si>
+    <t>Beziehung </t>
   </si>
 </sst>
 </file>
@@ -444,7 +441,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,7 +462,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -473,7 +470,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -481,7 +478,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -489,7 +486,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -497,7 +494,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -505,7 +502,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -513,7 +510,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -529,7 +526,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -537,7 +534,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -545,7 +542,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -553,7 +550,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -561,7 +558,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -569,7 +566,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -577,7 +574,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -585,7 +582,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -593,7 +590,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -601,7 +598,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -649,7 +646,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B25">
         <v>3</v>

</xml_diff>